<commit_message>
chore(scores): added missing week scores
</commit_message>
<xml_diff>
--- a/content/_data/NFL 2022 week 9.xlsx
+++ b/content/_data/NFL 2022 week 9.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="97">
   <si>
     <t xml:space="preserve">                               SPREAD POOL 2022</t>
   </si>
@@ -201,6 +201,9 @@
     <t>balt  -2 1/2  N.O.</t>
   </si>
   <si>
+    <t>40 pts.</t>
+  </si>
+  <si>
     <t>**Standings**</t>
   </si>
   <si>
@@ -234,7 +237,7 @@
     <t>CHRIS B</t>
   </si>
   <si>
-    <t>*after week 8*</t>
+    <t>*after week 9*</t>
   </si>
   <si>
     <t>pts</t>
@@ -243,25 +246,37 @@
     <t>PHIL**</t>
   </si>
   <si>
+    <t xml:space="preserve">BIG MAC </t>
+  </si>
+  <si>
     <t>Imbatman (1)</t>
   </si>
   <si>
-    <t xml:space="preserve">BIG MAC </t>
-  </si>
-  <si>
     <t>COSMO (1)</t>
   </si>
   <si>
     <t>CIN**</t>
   </si>
   <si>
+    <t>RAW (1.5)</t>
+  </si>
+  <si>
+    <t>KEN(1)</t>
+  </si>
+  <si>
+    <t>N..E.</t>
+  </si>
+  <si>
+    <t>the BEAR (1.5)</t>
+  </si>
+  <si>
     <t>KOLI (1)</t>
   </si>
   <si>
-    <t>N..E.</t>
-  </si>
-  <si>
-    <t>KEN(1)</t>
+    <t xml:space="preserve">TODD   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOLLYWOOD! </t>
   </si>
   <si>
     <t xml:space="preserve">DOG  </t>
@@ -270,21 +285,9 @@
     <t>T-ROD (1)</t>
   </si>
   <si>
-    <t xml:space="preserve">TODD   </t>
-  </si>
-  <si>
-    <t>RAW (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOLLYWOOD! </t>
-  </si>
-  <si>
     <t>CHRIS W (1)</t>
   </si>
   <si>
-    <t>the BEAR (1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">RYAN </t>
   </si>
   <si>
@@ -297,13 +300,13 @@
     <t xml:space="preserve">D'Alicia </t>
   </si>
   <si>
+    <t xml:space="preserve">ROCKET </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J-MAC </t>
+  </si>
+  <si>
     <t xml:space="preserve">CHRIS B </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROCKET </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J-MAC </t>
   </si>
   <si>
     <r>
@@ -312,7 +315,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="2"/>
       </rPr>
@@ -325,7 +328,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,14 +337,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="20"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -354,27 +363,27 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -386,13 +395,13 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -411,7 +420,7 @@
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -729,196 +738,202 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="13" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="14" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="21" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="13" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="21" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1234,27 +1249,27 @@
     <col min="1" max="1" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="63" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="64" width="0.8621428571428571" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="63" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="64" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="63" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="64" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="64" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="64" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="64" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="64" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="64" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="64" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="64" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="64" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="64" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="64" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="64" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="64" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="64" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="65" width="0.8621428571428571" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="64" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="65" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="64" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="65" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="66" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="66" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="66" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="66" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="66" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="66" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1279,7 +1294,7 @@
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="24.75">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1324,7 +1339,7 @@
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="23.25">
       <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
@@ -1356,11 +1371,15 @@
         <v>12</v>
       </c>
       <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
+      <c r="L3" s="18">
+        <v>29</v>
+      </c>
       <c r="M3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="20"/>
+      <c r="N3" s="20">
+        <v>17</v>
+      </c>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -1369,7 +1388,7 @@
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="23.25">
       <c r="A4" s="21" t="s">
         <v>15</v>
       </c>
@@ -1401,11 +1420,15 @@
         <v>15</v>
       </c>
       <c r="K4" s="17"/>
-      <c r="L4" s="18"/>
+      <c r="L4" s="18">
+        <v>20</v>
+      </c>
       <c r="M4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="20"/>
+      <c r="N4" s="20">
+        <v>17</v>
+      </c>
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
@@ -1414,7 +1437,7 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="23.25">
       <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
@@ -1446,11 +1469,15 @@
         <v>18</v>
       </c>
       <c r="K5" s="17"/>
-      <c r="L5" s="18"/>
+      <c r="L5" s="18">
+        <v>35</v>
+      </c>
       <c r="M5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="20"/>
+      <c r="N5" s="20">
+        <v>32</v>
+      </c>
       <c r="O5" s="15"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -1459,7 +1486,7 @@
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="23.25">
       <c r="A6" s="16" t="s">
         <v>22</v>
       </c>
@@ -1491,11 +1518,15 @@
         <v>23</v>
       </c>
       <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
+      <c r="L6" s="18">
+        <v>42</v>
+      </c>
       <c r="M6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="20"/>
+      <c r="N6" s="20">
+        <v>21</v>
+      </c>
       <c r="O6" s="15"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -1504,7 +1535,7 @@
       <c r="T6" s="6"/>
       <c r="U6" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="23.25">
       <c r="A7" s="16" t="s">
         <v>25</v>
       </c>
@@ -1536,11 +1567,15 @@
         <v>27</v>
       </c>
       <c r="K7" s="17"/>
-      <c r="L7" s="18"/>
+      <c r="L7" s="18">
+        <v>15</v>
+      </c>
       <c r="M7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="22"/>
+      <c r="N7" s="22">
+        <v>19</v>
+      </c>
       <c r="O7" s="15"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -1549,7 +1584,7 @@
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="23.25">
       <c r="A8" s="21" t="s">
         <v>29</v>
       </c>
@@ -1581,11 +1616,15 @@
         <v>30</v>
       </c>
       <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
+      <c r="L8" s="18">
+        <v>26</v>
+      </c>
       <c r="M8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="20"/>
+      <c r="N8" s="20">
+        <v>3</v>
+      </c>
       <c r="O8" s="15"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
@@ -1596,7 +1635,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="23.25">
       <c r="A9" s="16" t="s">
         <v>34</v>
       </c>
@@ -1628,11 +1667,15 @@
         <v>36</v>
       </c>
       <c r="K9" s="17"/>
-      <c r="L9" s="18"/>
+      <c r="L9" s="18">
+        <v>17</v>
+      </c>
       <c r="M9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="22"/>
+      <c r="N9" s="22">
+        <v>20</v>
+      </c>
       <c r="O9" s="15"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
@@ -1641,7 +1684,7 @@
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="23.25">
       <c r="A10" s="16" t="s">
         <v>38</v>
       </c>
@@ -1673,11 +1716,15 @@
         <v>38</v>
       </c>
       <c r="K10" s="17"/>
-      <c r="L10" s="18"/>
+      <c r="L10" s="18">
+        <v>20</v>
+      </c>
       <c r="M10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="20"/>
+      <c r="N10" s="20">
+        <v>17</v>
+      </c>
       <c r="O10" s="15"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
@@ -1686,7 +1733,7 @@
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="23.25">
       <c r="A11" s="21" t="s">
         <v>42</v>
       </c>
@@ -1718,11 +1765,15 @@
         <v>43</v>
       </c>
       <c r="K11" s="17"/>
-      <c r="L11" s="18"/>
+      <c r="L11" s="18">
+        <v>20</v>
+      </c>
       <c r="M11" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N11" s="22"/>
+      <c r="N11" s="22">
+        <v>27</v>
+      </c>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -1731,7 +1782,7 @@
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="23.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1754,7 +1805,7 @@
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="23.25">
       <c r="A13" s="21" t="s">
         <v>46</v>
       </c>
@@ -1786,11 +1837,15 @@
         <v>47</v>
       </c>
       <c r="K13" s="17"/>
-      <c r="L13" s="18"/>
+      <c r="L13" s="18">
+        <v>21</v>
+      </c>
       <c r="M13" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="N13" s="22"/>
+      <c r="N13" s="22">
+        <v>31</v>
+      </c>
       <c r="O13" s="15"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
@@ -1799,7 +1854,7 @@
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="23.25">
       <c r="A14" s="16" t="s">
         <v>50</v>
       </c>
@@ -1831,11 +1886,15 @@
         <v>51</v>
       </c>
       <c r="K14" s="17"/>
-      <c r="L14" s="18"/>
+      <c r="L14" s="18">
+        <v>16</v>
+      </c>
       <c r="M14" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="N14" s="20"/>
+      <c r="N14" s="20">
+        <v>13</v>
+      </c>
       <c r="O14" s="15"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
@@ -1844,7 +1903,7 @@
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="23.25">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1867,7 +1926,7 @@
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="23.25">
       <c r="A16" s="16" t="s">
         <v>53</v>
       </c>
@@ -1899,11 +1958,15 @@
         <v>53</v>
       </c>
       <c r="K16" s="17"/>
-      <c r="L16" s="18"/>
+      <c r="L16" s="18">
+        <v>20</v>
+      </c>
       <c r="M16" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="N16" s="20"/>
+      <c r="N16" s="20">
+        <v>17</v>
+      </c>
       <c r="O16" s="15"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
@@ -1912,7 +1975,7 @@
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="23.25">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -1935,7 +1998,7 @@
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="23.25">
       <c r="A18" s="16" t="s">
         <v>56</v>
       </c>
@@ -1967,11 +2030,15 @@
         <v>56</v>
       </c>
       <c r="K18" s="17"/>
-      <c r="L18" s="18"/>
+      <c r="L18" s="18">
+        <v>27</v>
+      </c>
       <c r="M18" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="20"/>
+      <c r="N18" s="20">
+        <v>13</v>
+      </c>
       <c r="O18" s="15"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
@@ -1980,7 +2047,7 @@
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="23.25">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1993,7 +2060,9 @@
       <c r="J19" s="16"/>
       <c r="K19" s="17"/>
       <c r="L19" s="18"/>
-      <c r="M19" s="19"/>
+      <c r="M19" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="N19" s="20"/>
       <c r="O19" s="15"/>
       <c r="P19" s="6"/>
@@ -2003,7 +2072,7 @@
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="23.25">
       <c r="A20" s="24">
         <v>46</v>
       </c>
@@ -2046,7 +2115,7 @@
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="24.95">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="23.25">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -2154,7 +2223,7 @@
       <c r="K25" s="36"/>
       <c r="L25" s="37"/>
       <c r="M25" s="38" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N25" s="35"/>
       <c r="O25" s="15"/>
@@ -2167,42 +2236,42 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="21.75">
       <c r="A26" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K26" s="17"/>
       <c r="L26" s="39"/>
       <c r="M26" s="40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N26" s="41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O26" s="15"/>
       <c r="P26" s="6"/>
@@ -2223,7 +2292,7 @@
         <v>12</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>12</v>
@@ -2248,10 +2317,10 @@
         <v>1</v>
       </c>
       <c r="M27" s="43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N27" s="44">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="O27" s="15"/>
       <c r="P27" s="6"/>
@@ -2297,10 +2366,10 @@
         <v>2</v>
       </c>
       <c r="M28" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N28" s="44">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="O28" s="15"/>
       <c r="P28" s="6"/>
@@ -2346,10 +2415,10 @@
         <v>3</v>
       </c>
       <c r="M29" s="46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N29" s="48">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="O29" s="15"/>
       <c r="P29" s="6"/>
@@ -2364,7 +2433,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>22</v>
@@ -2392,13 +2461,13 @@
       </c>
       <c r="K30" s="17"/>
       <c r="L30" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M30" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="N30" s="48">
         <v>78</v>
-      </c>
-      <c r="N30" s="48">
-        <v>70</v>
       </c>
       <c r="O30" s="15"/>
       <c r="P30" s="6"/>
@@ -2441,13 +2510,13 @@
       </c>
       <c r="K31" s="17"/>
       <c r="L31" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M31" s="46" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="N31" s="44">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="O31" s="15"/>
       <c r="P31" s="6"/>
@@ -2477,7 +2546,7 @@
         <v>29</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H32" s="21" t="s">
         <v>29</v>
@@ -2493,10 +2562,10 @@
         <v>6</v>
       </c>
       <c r="M32" s="46" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="N32" s="50">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="O32" s="15"/>
       <c r="P32" s="6"/>
@@ -2539,13 +2608,13 @@
       </c>
       <c r="K33" s="17"/>
       <c r="L33" s="45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M33" s="46" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N33" s="48">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="O33" s="15"/>
       <c r="P33" s="6"/>
@@ -2588,13 +2657,13 @@
       </c>
       <c r="K34" s="17"/>
       <c r="L34" s="49">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M34" s="46" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N34" s="48">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="O34" s="15"/>
       <c r="P34" s="6"/>
@@ -2637,13 +2706,13 @@
       </c>
       <c r="K35" s="17"/>
       <c r="L35" s="45">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M35" s="46" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N35" s="48">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="O35" s="15"/>
       <c r="P35" s="6"/>
@@ -2666,13 +2735,13 @@
       <c r="J36" s="21"/>
       <c r="K36" s="17"/>
       <c r="L36" s="49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M36" s="46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N36" s="44">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="O36" s="15"/>
       <c r="P36" s="6"/>
@@ -2718,10 +2787,10 @@
         <v>11</v>
       </c>
       <c r="M37" s="51" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N37" s="48">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="O37" s="15"/>
       <c r="P37" s="6"/>
@@ -2767,10 +2836,10 @@
         <v>12</v>
       </c>
       <c r="M38" s="46" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N38" s="44">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="O38" s="15"/>
       <c r="P38" s="6"/>
@@ -2793,13 +2862,13 @@
       <c r="J39" s="16"/>
       <c r="K39" s="17"/>
       <c r="L39" s="45">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M39" s="46" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N39" s="48">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O39" s="15"/>
       <c r="P39" s="6"/>
@@ -2845,10 +2914,10 @@
         <v>14</v>
       </c>
       <c r="M40" s="46" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N40" s="53">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="O40" s="15"/>
       <c r="P40" s="6"/>
@@ -2871,13 +2940,13 @@
       <c r="J41" s="16"/>
       <c r="K41" s="17"/>
       <c r="L41" s="45">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M41" s="46" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N41" s="44">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="O41" s="15"/>
       <c r="P41" s="6"/>
@@ -2916,17 +2985,17 @@
         <v>56</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K42" s="54"/>
       <c r="L42" s="45">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M42" s="55" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N42" s="44">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="O42" s="15"/>
       <c r="P42" s="6"/>
@@ -2955,7 +3024,7 @@
         <v>10</v>
       </c>
       <c r="N43" s="44">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="O43" s="15"/>
       <c r="P43" s="6"/>
@@ -2998,13 +3067,13 @@
       </c>
       <c r="K44" s="30"/>
       <c r="L44" s="49">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M44" s="46" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N44" s="48">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="O44" s="15"/>
       <c r="P44" s="6"/>
@@ -3030,10 +3099,10 @@
         <v>19</v>
       </c>
       <c r="M45" s="46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N45" s="44">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="O45" s="15"/>
       <c r="P45" s="6"/>
@@ -3059,10 +3128,10 @@
         <v>20</v>
       </c>
       <c r="M46" s="46" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N46" s="48">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="O46" s="15"/>
       <c r="P46" s="6"/>
@@ -3159,7 +3228,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="60"/>
       <c r="M50" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N50" s="60"/>
       <c r="O50" s="5"/>

</xml_diff>